<commit_message>
begin to examine the disconnection
</commit_message>
<xml_diff>
--- a/excel/Different settings.xlsx
+++ b/excel/Different settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Pacific\1科研\57trans拓扑辨识理论极限\distribution_system_identification_theoretical_limit\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB56E13-20BA-440C-91FD-E381ACD82C1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615E1837-1635-4301-91F8-6ACAAE8DF242}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="8390" xr2:uid="{0BA08903-BDD7-4BC6-AFAE-73BB1CC1A755}"/>
   </bookViews>
@@ -87,7 +87,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>failure</t>
+    <t>fail</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -455,7 +455,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -514,10 +514,10 @@
         <v>13</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>4.0045049586666468E-3</v>
@@ -542,6 +542,9 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -559,6 +562,18 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
+      <c r="F4">
+        <v>3.125</v>
+      </c>
+      <c r="G4">
+        <v>3.125</v>
+      </c>
+      <c r="H4">
+        <v>1.0631716963287633E-2</v>
+      </c>
+      <c r="I4">
+        <v>5.6566983573779128E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -577,10 +592,10 @@
         <v>6</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>1.2092046502352616</v>
@@ -643,10 +658,10 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>3.7169147867118628</v>
@@ -672,10 +687,10 @@
         <v>6</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>34.421132776214343</v>

</xml_diff>

<commit_message>
current version without detecting disconnection
</commit_message>
<xml_diff>
--- a/excel/Different settings.xlsx
+++ b/excel/Different settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Pacific\1科研\57trans拓扑辨识理论极限\distribution_system_identification_theoretical_limit\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615E1837-1635-4301-91F8-6ACAAE8DF242}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70252BF2-6C68-43B2-A1F0-2DDE117E531D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="8390" xr2:uid="{0BA08903-BDD7-4BC6-AFAE-73BB1CC1A755}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -542,9 +542,6 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -620,9 +617,6 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -639,6 +633,9 @@
       </c>
       <c r="E7" t="s">
         <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>